<commit_message>
Anpassung an GAFs und Anforderungsliste
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_Anforderungsliste.xlsx
+++ b/Doku/Stundenplan_Anforderungsliste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-60" yWindow="20" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nicht-funktional" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Alle Daten werden in einer relationalen Datenbank gespeichert.</t>
   </si>
@@ -34,9 +34,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Anforderungstyp</t>
-  </si>
-  <si>
     <t>BUC</t>
   </si>
   <si>
@@ -65,6 +62,113 @@
   </si>
   <si>
     <t>Änderungen</t>
+  </si>
+  <si>
+    <t>BUC2</t>
+  </si>
+  <si>
+    <t>Begründung</t>
+  </si>
+  <si>
+    <t>Das System muss einen entsprechenden Eingabedialog aufweisen.</t>
+  </si>
+  <si>
+    <t>Wichtigkeit (0 - 5)</t>
+  </si>
+  <si>
+    <t>Das System soll dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen.</t>
+  </si>
+  <si>
+    <t>Das System wird dem Benutzer keine Möglichkeit bieten die Stammdaten zu editieren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Steigerung der Usability.
+ - Eine Zeitpräferenz wie zum Beispiel Vormittags ist sehr ungenau. Die Erfassung in vordefinierten Zeitblöcken verbessert das Planungsergebnis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Die Stammdaten der zu erfassenden Studiengänge, Räume oder Dozenten verändert sich nur geringfügig. Den Benutzern soll aus diesem Grund keine Anpassungs-möglichkeit gewährt werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Das System darf keinen Eingabedialog auf Stammdaten zulassen.
+ - Das System darf keinen schreibenden Zugriff auf Tabellen der Stammdaten gewähren.</t>
+  </si>
+  <si>
+    <t>Das System soll den Benutzer bei der Aufnahme einer Zeitpräferenz, welche bereits X-Mal vergeben wurde, warnen und Zeitvorschläge unterbreiten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Es stehen nur begrenzte Räumlichkeiten zur Verfügung. Veranstaltungen müssen dementsprechend abgestimmt werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Keine zusätzliche Installation auf den Client-Arbeitsplätzen.</t>
+  </si>
+  <si>
+    <t>Der Aufruf und die Bearbeitung des Stundenplanerstellungstools ist über einen beliebigen Browser möglich.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Zentrale Speicherung jeglicher relevanter Daten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Höhere Skalierbarkeit.
+ - Höhere Sicherheit.
+ - Bessere Trennung der einzelnen Komponenten.</t>
+  </si>
+  <si>
+    <t>Sobald ein Benutzer das Planungsmodul aufruft, muss dieses innerhalb von 2 Sekunden vollständig zur Verfügung stehen.</t>
+  </si>
+  <si>
+    <t>Ein Benutzer muss nach 30 minütiger Einarbeitungszeit in der Lage sein, die Zeitpräferenzen eines Dozenten zu erfassen.</t>
+  </si>
+  <si>
+    <t>Fehlertoleranz</t>
+  </si>
+  <si>
+    <t>Robustheit</t>
+  </si>
+  <si>
+    <t>Bedienbarkeit</t>
+  </si>
+  <si>
+    <t>Dem Benutzer muss die Möglichkeit gewährt werden jegliche Eingaben über die Tastatur oder die Maus vorzunehmen.</t>
+  </si>
+  <si>
+    <t>Zeitverhalten</t>
+  </si>
+  <si>
+    <t>Verbrauchsverhalten</t>
+  </si>
+  <si>
+    <t>Analysierbarkeit</t>
+  </si>
+  <si>
+    <t>Modifizierbarkeit</t>
+  </si>
+  <si>
+    <t>Stabilität</t>
+  </si>
+  <si>
+    <t>Testbarkeit</t>
+  </si>
+  <si>
+    <t>Anpassbarkeit</t>
+  </si>
+  <si>
+    <t>Installierbarkeit</t>
+  </si>
+  <si>
+    <t>Koexistenz</t>
+  </si>
+  <si>
+    <t>BUC1</t>
+  </si>
+  <si>
+    <t>Das System muss das mathematische Zuordnungsproblem der vorhandenen Informationen (Raum, Veranstaltung, Dozent inklusive Zeitpräferenz) mit Hilfe eines geeigneten Algorithmus automatisch berechnen.</t>
+  </si>
+  <si>
+    <t>Das System muss infolge der Berechnung eine zulässige Lösung anzeigen und die Möglichkeit zur Speicherung bereitstellen.</t>
+  </si>
+  <si>
+    <t>Das System sollte dem Benutzer, im Zuge einer automatischen Planung und im Nachlauf einer bereits durchgeführten Planung, eine Rückfrage liefern ob die Planung der bestehenden Planung angefügt werden  oder eine neue Planung erstellt werden soll.
+Oder Hinweis auf Verlust der Daten bei zweitmaliger Ausführung.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,19 +252,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -493,73 +642,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="53" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="55.5" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6" style="6" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="30">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="D3" s="1" t="s">
+      <c r="D2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="60">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="75">
-      <c r="D4" s="1" t="s">
+      <c r="D3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="75">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="30">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="30">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" s="11" customFormat="1" ht="30">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" s="11" customFormat="1">
+      <c r="A8" s="10"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" s="11" customFormat="1">
+      <c r="A9" s="10"/>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" s="11" customFormat="1">
+      <c r="A10" s="10"/>
+      <c r="C10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" s="11" customFormat="1">
+      <c r="A11" s="10"/>
+      <c r="C11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" s="11" customFormat="1">
+      <c r="A12" s="10"/>
+      <c r="C12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" s="11" customFormat="1">
+      <c r="A13" s="10"/>
+      <c r="C13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" s="11" customFormat="1">
+      <c r="A14" s="10"/>
+      <c r="C14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" s="11" customFormat="1">
+      <c r="A15" s="10"/>
+      <c r="C15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" s="11" customFormat="1">
+      <c r="A16" s="10"/>
+      <c r="C16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="11" customFormat="1">
+      <c r="A17" s="10"/>
+      <c r="C17" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="11" customFormat="1">
+      <c r="A18" s="10"/>
+      <c r="C18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="11" customFormat="1">
+      <c r="A19" s="10"/>
+      <c r="C19" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" s="11" customFormat="1">
+      <c r="A20" s="10"/>
+      <c r="C20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" s="11" customFormat="1">
+      <c r="A21" s="10"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="11" customFormat="1">
+      <c r="A22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" s="11" customFormat="1">
+      <c r="A23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" s="11" customFormat="1">
+      <c r="A24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" s="11" customFormat="1">
+      <c r="A25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" s="11" customFormat="1">
+      <c r="A26" s="10"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="11" customFormat="1">
+      <c r="A27" s="10"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" s="11" customFormat="1">
+      <c r="A28" s="10"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" s="11" customFormat="1">
+      <c r="A29" s="10"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" s="11" customFormat="1">
+      <c r="A30" s="10"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" s="11" customFormat="1">
+      <c r="A31" s="10"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" s="11" customFormat="1">
+      <c r="A32" s="10"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="1:6" s="11" customFormat="1">
+      <c r="A33" s="10"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="1:6" s="11" customFormat="1">
+      <c r="A34" s="10"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="1:6" s="11" customFormat="1">
+      <c r="A35" s="10"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" s="11" customFormat="1">
+      <c r="A36" s="10"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" s="11" customFormat="1">
+      <c r="A37" s="10"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" s="11" customFormat="1">
+      <c r="A38" s="10"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" s="4" customFormat="1">
+      <c r="A39" s="6"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" s="4" customFormat="1">
+      <c r="A40" s="6"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" s="4" customFormat="1">
+      <c r="A41" s="6"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" s="4" customFormat="1">
+      <c r="A42" s="6"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" s="4" customFormat="1">
+      <c r="A43" s="6"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" s="4" customFormat="1">
+      <c r="A44" s="6"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" s="4" customFormat="1">
+      <c r="A45" s="6"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" s="4" customFormat="1">
+      <c r="A46" s="6"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" s="4" customFormat="1">
+      <c r="A47" s="6"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="F47" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -574,65 +1037,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="90">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="105">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="75">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="120">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="C7" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Bearbeitung GAF und Anforderungen
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_Anforderungsliste.xlsx
+++ b/Doku/Stundenplan_Anforderungsliste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nicht-funktional" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
   <si>
     <t>Alle Daten werden in einer relationalen Datenbank gespeichert.</t>
   </si>
@@ -67,13 +67,7 @@
     <t>Begründung</t>
   </si>
   <si>
-    <t>Das System muss einen entsprechenden Eingabedialog aufweisen.</t>
-  </si>
-  <si>
     <t>Wichtigkeit (0 - 5)</t>
-  </si>
-  <si>
-    <t>Das System soll dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen.</t>
   </si>
   <si>
     <t>Das System wird dem Benutzer keine Möglichkeit bieten die Stammdaten zu editieren.</t>
@@ -149,9 +143,6 @@
     <t>Das System muss das mathematische Zuordnungsproblem der vorhandenen Informationen (Raum, Veranstaltung, Dozent inklusive Zeitpräferenz) mit Hilfe eines geeigneten Algorithmus automatisch berechnen.</t>
   </si>
   <si>
-    <t>Das System muss infolge der Berechnung eine zulässige Lösung anzeigen und die Möglichkeit zur Speicherung bereitstellen.</t>
-  </si>
-  <si>
     <t>Das System sollte dem Benutzer, im Zuge einer automatischen Planung und im Nachlauf einer bereits durchgeführten Planung, eine Rückfrage liefern ob die Planung der bestehenden Planung angefügt werden  oder eine neue Planung erstellt werden soll.
 Oder Hinweis auf Verlust der Daten bei zweitmaliger Ausführung.</t>
   </si>
@@ -187,13 +178,130 @@
   </si>
   <si>
     <t>Abstürze, Absturzursachen</t>
+  </si>
+  <si>
+    <t>Das System muss dem Benutzer die Möglichkeit bieten die Planung manuell, durch Auswahl eines Feldes, als abgeschlossen zu markieren.</t>
+  </si>
+  <si>
+    <t>Das System muss dem Benutzer bei Auswahl des Feldes "Planung abgeschlossen" eine Rückmeldung liefern, dass die Planung für das jeweilige Semester anschließend nicht mehr verändert werden kann.</t>
+  </si>
+  <si>
+    <t>Das System soll in der Zeiterfassungsmaske einen Dozenten, dessen Zeitpräferenzen bereits erfasst sind, als "erfasst" markieren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Steigerung der Usability.</t>
+  </si>
+  <si>
+    <t>Das System soll einen entsprechenden Eingabedialog aufweisen.</t>
+  </si>
+  <si>
+    <t>Das System soll über einen RadioButton verfügen, der die Erfassung kennzeichnet.</t>
+  </si>
+  <si>
+    <t>Das System soll bereits erfasste Zeitpräferenzen eines Dozenten, bei erneuten Aufruf der jeweiligen Zeiterfassung, durch Markierung der vordefinierten Zeitblöcke visualisieren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Sichtbarmachung der bisher getätigten Zeitaufnahmen.
+ - Steigerung der Usability.</t>
+  </si>
+  <si>
+    <t>Das System soll dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen und speichern.</t>
+  </si>
+  <si>
+    <t>Das System soll die Zeiten eines Dozenten in dem entsprechenden Eingabedialog anzeigen.</t>
+  </si>
+  <si>
+    <t>Das System soll dem Benutzer die Möglichkeit bieten jegliche Zeitpräferenzen eines Dozenten mit einem Klick zu entfernen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Steigerung der Usability.
+ - Vereinfachung der Bearbeitung eines Dozenten (Zeitpräferenzen).</t>
+  </si>
+  <si>
+    <t>"Leeren" Button, der die Zeitpräferenzen entfernt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Eine manuelle Zuteilung der einzelnen Dozenten inklusive ihrer Zeitpräferenzen zu bestehenden Räumen und Modulen ist zu aufwendig und zu zeitintensiv</t>
+  </si>
+  <si>
+    <t>Das System muss infolge der Berechnung eine zulässige Lösung anzeigen können und diese Lösung automatisch abspeichern.</t>
+  </si>
+  <si>
+    <t>Das System soll dem Benutzer die Möglichkeit bieten den Stundenplan der aktuellen Semesterplanung manuell anzupassen.</t>
+  </si>
+  <si>
+    <t>Ein Dialog zur Änderung einzelner Blöcke.</t>
+  </si>
+  <si>
+    <t>Das System soll bei manueller Anpassung einzelner Blöcke mit anschließenden Kollisionen Zuordnungsvorschläge (Raum und Zeit) unterbreiten.</t>
+  </si>
+  <si>
+    <t>Das System soll eine automatische Planung auch ohne die Erfassung aller Zeitpräferenzen ermöglichen.</t>
+  </si>
+  <si>
+    <t>Das System soll eine Hinweismeldung ausgeben, falls eine Planung gestartet wird und nicht alle Zeiten erfasst wurden.</t>
+  </si>
+  <si>
+    <t>Nach der Ausführung der automatischen Planung, muss über die Anzeige ein vollständiger Stundenplan aufrufbar sein.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Ein regelmäßiger Zugriff auf die erstellten Daten ist notwendig.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Um fehlerhafte Planungen zu korrigieren.</t>
+  </si>
+  <si>
+    <t>Button durch den eine bestehende Planung gelöscht wird.</t>
+  </si>
+  <si>
+    <t>BUC4</t>
+  </si>
+  <si>
+    <t>Das System muss die Möglichkeit bieten, solange die Planung nicht als abgeschlossen markiert wurde, die gesamte Planung manuell zu löschen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Wenn das Semester begonnen hat, darf die Planung nicht mehr grundlegend verändert werden.</t>
+  </si>
+  <si>
+    <t>Button "Planung abschließen" der die Änderungen festschreibt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Einen versehentlichen Abschluss verhindern.</t>
+  </si>
+  <si>
+    <t>Rückmeldung vom System bevor der Abschluss gesetzt wird.</t>
+  </si>
+  <si>
+    <t>BUC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Einzelne Änderung auf Basis menschlicher Erkenntnisse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Es können Zeiten oder Räume ausgewählt werden, die nicht zur Verfügung stehen.</t>
+  </si>
+  <si>
+    <t>Nur relevant, wenn nicht ausschließlich freie Bläcke zu sehen sind</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Dozenten lassen sich mit der Zeitvergabe Zeit.
+ - Erste Planung zur Prüfung von Kollisionen.</t>
+  </si>
+  <si>
+    <t>Stundenplan wird mit vergebenen Informationen erstellt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Versehentliche Planung verhindern.</t>
+  </si>
+  <si>
+    <t>Hinweismeldung ausgeben.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +339,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -261,8 +376,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -338,17 +459,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="37">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -364,6 +485,9 @@
     <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -379,6 +503,9 @@
     <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,7 +837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -766,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" s="12"/>
     </row>
@@ -775,13 +902,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" ht="75">
@@ -792,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="12"/>
     </row>
@@ -801,10 +928,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -813,10 +940,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -825,10 +952,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="12"/>
     </row>
@@ -837,10 +964,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -849,10 +976,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="12"/>
     </row>
@@ -861,10 +988,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -881,47 +1008,47 @@
     <row r="13" spans="1:11" s="11" customFormat="1">
       <c r="A13" s="10"/>
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:11" s="11" customFormat="1">
       <c r="A14" s="10"/>
       <c r="C14" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:11" s="11" customFormat="1">
       <c r="A15" s="10"/>
       <c r="C15" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:11" s="11" customFormat="1">
       <c r="A16" s="10"/>
       <c r="C16" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1">
       <c r="A17" s="10"/>
       <c r="C17" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="12"/>
       <c r="F17" s="12"/>
@@ -929,7 +1056,7 @@
     <row r="18" spans="1:6" s="11" customFormat="1">
       <c r="A18" s="10"/>
       <c r="C18" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="12"/>
       <c r="F18" s="12"/>
@@ -1120,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1162,7 +1289,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>9</v>
@@ -1185,74 +1312,216 @@
         <v>13</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>19</v>
-      </c>
       <c r="F2" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="105">
-      <c r="A3" s="11">
-        <v>2</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45">
+      <c r="B3" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="75">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60">
       <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="75">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45">
       <c r="B5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="15" customFormat="1" ht="75">
+      <c r="B6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="8" spans="1:11" ht="75">
+      <c r="B8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="75">
+      <c r="B9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="15" customFormat="1" ht="120">
+      <c r="C10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="45">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="15" customFormat="1" ht="120">
-      <c r="A7" s="15">
-        <v>6</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="D10" s="16"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" ht="45">
+      <c r="B11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45">
+      <c r="B12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60">
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45">
+      <c r="B14" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="15" customFormat="1" ht="45">
+      <c r="B15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="H15" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="60">
+      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="45">
+      <c r="B17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="105">
+      <c r="C18" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="11">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Anpassung Anforderungen, GAFs, Stakeholder, Ziel
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_Anforderungsliste.xlsx
+++ b/Doku/Stundenplan_Anforderungsliste.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="nicht-funktional" sheetId="1" r:id="rId1"/>
-    <sheet name="funktional" sheetId="2" r:id="rId2"/>
+    <sheet name="funktional" sheetId="2" r:id="rId1"/>
+    <sheet name="nicht-funktional" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
   <si>
     <t>Alle Daten werden in einer relationalen Datenbank gespeichert.</t>
   </si>
@@ -71,10 +71,6 @@
   </si>
   <si>
     <t>Das System wird dem Benutzer keine Möglichkeit bieten die Stammdaten zu editieren.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Steigerung der Usability.
- - Eine Zeitpräferenz wie zum Beispiel Vormittags ist sehr ungenau. Die Erfassung in vordefinierten Zeitblöcken verbessert das Planungsergebnis.</t>
   </si>
   <si>
     <t xml:space="preserve"> - Die Stammdaten der zu erfassenden Studiengänge, Räume oder Dozenten verändert sich nur geringfügig. Den Benutzern soll aus diesem Grund keine Anpassungs-möglichkeit gewährt werden.</t>
@@ -85,9 +81,6 @@
   </si>
   <si>
     <t>Das System soll den Benutzer bei der Aufnahme einer Zeitpräferenz, welche bereits X-Mal vergeben wurde, warnen und Zeitvorschläge unterbreiten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Es stehen nur begrenzte Räumlichkeiten zur Verfügung. Veranstaltungen müssen dementsprechend abgestimmt werden.</t>
   </si>
   <si>
     <t>Der Aufruf und die Bearbeitung des Stundenplanerstellungstools ist über einen beliebigen Browser möglich.</t>
@@ -143,10 +136,6 @@
     <t>Das System muss das mathematische Zuordnungsproblem der vorhandenen Informationen (Raum, Veranstaltung, Dozent inklusive Zeitpräferenz) mit Hilfe eines geeigneten Algorithmus automatisch berechnen.</t>
   </si>
   <si>
-    <t>Das System sollte dem Benutzer, im Zuge einer automatischen Planung und im Nachlauf einer bereits durchgeführten Planung, eine Rückfrage liefern ob die Planung der bestehenden Planung angefügt werden  oder eine neue Planung erstellt werden soll.
-Oder Hinweis auf Verlust der Daten bei zweitmaliger Ausführung.</t>
-  </si>
-  <si>
     <t>Das System muss dem Benutzer die Möglichkeit gewähren jegliche Eingaben über die Tastatur oder die Maus vorzunehmen.</t>
   </si>
   <si>
@@ -186,47 +175,19 @@
     <t>Das System muss dem Benutzer bei Auswahl des Feldes "Planung abgeschlossen" eine Rückmeldung liefern, dass die Planung für das jeweilige Semester anschließend nicht mehr verändert werden kann.</t>
   </si>
   <si>
-    <t>Das System soll in der Zeiterfassungsmaske einen Dozenten, dessen Zeitpräferenzen bereits erfasst sind, als "erfasst" markieren.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Steigerung der Usability.</t>
-  </si>
-  <si>
     <t>Das System soll einen entsprechenden Eingabedialog aufweisen.</t>
-  </si>
-  <si>
-    <t>Das System soll über einen RadioButton verfügen, der die Erfassung kennzeichnet.</t>
-  </si>
-  <si>
-    <t>Das System soll bereits erfasste Zeitpräferenzen eines Dozenten, bei erneuten Aufruf der jeweiligen Zeiterfassung, durch Markierung der vordefinierten Zeitblöcke visualisieren.</t>
   </si>
   <si>
     <t xml:space="preserve"> - Sichtbarmachung der bisher getätigten Zeitaufnahmen.
  - Steigerung der Usability.</t>
   </si>
   <si>
-    <t>Das System soll dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen und speichern.</t>
-  </si>
-  <si>
     <t>Das System soll die Zeiten eines Dozenten in dem entsprechenden Eingabedialog anzeigen.</t>
   </si>
   <si>
-    <t>Das System soll dem Benutzer die Möglichkeit bieten jegliche Zeitpräferenzen eines Dozenten mit einem Klick zu entfernen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Steigerung der Usability.
- - Vereinfachung der Bearbeitung eines Dozenten (Zeitpräferenzen).</t>
-  </si>
-  <si>
-    <t>"Leeren" Button, der die Zeitpräferenzen entfernt.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Eine manuelle Zuteilung der einzelnen Dozenten inklusive ihrer Zeitpräferenzen zu bestehenden Räumen und Modulen ist zu aufwendig und zu zeitintensiv</t>
   </si>
   <si>
-    <t>Das System muss infolge der Berechnung eine zulässige Lösung anzeigen können und diese Lösung automatisch abspeichern.</t>
-  </si>
-  <si>
     <t>Das System soll dem Benutzer die Möglichkeit bieten den Stundenplan der aktuellen Semesterplanung manuell anzupassen.</t>
   </si>
   <si>
@@ -236,18 +197,9 @@
     <t>Das System soll bei manueller Anpassung einzelner Blöcke mit anschließenden Kollisionen Zuordnungsvorschläge (Raum und Zeit) unterbreiten.</t>
   </si>
   <si>
-    <t>Das System soll eine automatische Planung auch ohne die Erfassung aller Zeitpräferenzen ermöglichen.</t>
-  </si>
-  <si>
-    <t>Das System soll eine Hinweismeldung ausgeben, falls eine Planung gestartet wird und nicht alle Zeiten erfasst wurden.</t>
-  </si>
-  <si>
     <t>Nach der Ausführung der automatischen Planung, muss über die Anzeige ein vollständiger Stundenplan aufrufbar sein.</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Ein regelmäßiger Zugriff auf die erstellten Daten ist notwendig.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Um fehlerhafte Planungen zu korrigieren.</t>
   </si>
   <si>
@@ -279,9 +231,6 @@
   </si>
   <si>
     <t xml:space="preserve"> - Es können Zeiten oder Räume ausgewählt werden, die nicht zur Verfügung stehen.</t>
-  </si>
-  <si>
-    <t>Nur relevant, wenn nicht ausschließlich freie Bläcke zu sehen sind</t>
   </si>
   <si>
     <t xml:space="preserve"> - Dozenten lassen sich mit der Zeitvergabe Zeit.
@@ -295,13 +244,104 @@
   </si>
   <si>
     <t>Hinweismeldung ausgeben.</t>
+  </si>
+  <si>
+    <t>hoch</t>
+  </si>
+  <si>
+    <t>Das System muss nach der Berechnung des Zuordnungsproblems eine zulässige Lösung in Form eines Stundenplans anzeigen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Die Berechnung des Stundenplans muss manuell einmalig, in Form von Stichproben, überprüft werden.</t>
+  </si>
+  <si>
+    <t>Nach der Ausführung der automatischen Planung muss automatisch ein Stundenplan angezeigt werden.</t>
+  </si>
+  <si>
+    <t>Das System muss dem Benutzer die Möglichkeit bieten die Ergebnisse der Stundenplanberechnung, durch die Betätigung eines "Speicher-Buttons", mit geeigneten Informationen in einer relationalen Datenbank festzuhalten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Eine durchgeführte Planung muss ggf. ein weiteres mal aufgerufen werden.</t>
+  </si>
+  <si>
+    <t>Nach der manuellen Speicherung, müssen die betreffenden Daten aus der Datenbank auslesbar sein.</t>
+  </si>
+  <si>
+    <t>Nur relevant wenn GAF "Planung löschen" aktiv ist.</t>
+  </si>
+  <si>
+    <t>Nur relevant wenn Planung manuell abgeschlossen werden soll.</t>
+  </si>
+  <si>
+    <t>Das System soll beim Start einer automatischen Planung eine bestehende Planung automatisch löschen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Eine Planung soll ohne Einschränkungen durchgeführt werden.</t>
+  </si>
+  <si>
+    <t>Eine bestehende Planung wird automatisch überschrieben.</t>
+  </si>
+  <si>
+    <t>Das System soll eine automatische Planung auch ohne die Erfassung aller Zeitpräferenzen, jedoch mit mindestens einer Zeitpräferenz, ermöglichen.</t>
+  </si>
+  <si>
+    <t>Das System kann eine Hinweismeldung ausgeben, falls eine Planung gestartet wird und nicht alle Dozenten die Zeitpräferenzen erfasst haben.</t>
+  </si>
+  <si>
+    <t>niedrig</t>
+  </si>
+  <si>
+    <t>mittel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Steigerung der Usability.
+ - Verbesserung des Planungsergebnis.</t>
+  </si>
+  <si>
+    <t>Das System muss dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten zu erfassen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Eine Lehrplanerstellung ermöglichen.</t>
+  </si>
+  <si>
+    <t>Möglichkeit zur Eingabe der Zeitpräferenzen geschaffen.</t>
+  </si>
+  <si>
+    <t>ID 7</t>
+  </si>
+  <si>
+    <t>ID 8</t>
+  </si>
+  <si>
+    <t>Opionaler GAF</t>
+  </si>
+  <si>
+    <t>Optionaler GAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Es stehen nur begrenzte Räumlichkeiten zur Verfügung. </t>
+  </si>
+  <si>
+    <t>Nur relevant wenn GAF "Planung manuell bearbeiten" aktiv ist.</t>
+  </si>
+  <si>
+    <t>Das System kann dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen und speichern.</t>
+  </si>
+  <si>
+    <t>Das System sollte dem Benutzer die Möglichkeit bieten bereits erfasste Zeitpräferenzen eines Dozenten anzeigen und bearbeiten zu können.</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>optionaler GAF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,8 +386,29 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,12 +418,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +431,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -414,8 +469,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -459,17 +540,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="63">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -488,6 +590,19 @@
     <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -506,6 +621,19 @@
     <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,9 +963,431 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="4.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="11">
+        <v>5</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="11">
+        <v>5</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="11">
+        <v>5</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="11">
+        <v>3</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="11">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="11">
+        <v>5</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="60">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="11">
+        <v>2</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="60">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="11">
+        <v>3</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="16" customFormat="1" ht="45">
+      <c r="B16" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="2:10" ht="45">
+      <c r="B17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="45">
+      <c r="C18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="60">
+      <c r="C19" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="45">
+      <c r="B20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" s="16" customFormat="1" ht="45">
+      <c r="B21" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="105">
+      <c r="C22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G20:I20"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -893,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="12"/>
     </row>
@@ -902,13 +1452,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" ht="75">
@@ -919,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="12"/>
     </row>
@@ -928,10 +1478,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -940,10 +1490,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -952,10 +1502,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="12"/>
     </row>
@@ -964,10 +1514,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -976,10 +1526,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="12"/>
     </row>
@@ -988,10 +1538,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -1008,47 +1558,47 @@
     <row r="13" spans="1:11" s="11" customFormat="1">
       <c r="A13" s="10"/>
       <c r="C13" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:11" s="11" customFormat="1">
       <c r="A14" s="10"/>
       <c r="C14" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:11" s="11" customFormat="1">
       <c r="A15" s="10"/>
       <c r="C15" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:11" s="11" customFormat="1">
       <c r="A16" s="10"/>
       <c r="C16" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" s="11" customFormat="1">
       <c r="A17" s="10"/>
       <c r="C17" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="12"/>
       <c r="F17" s="12"/>
@@ -1056,7 +1606,7 @@
     <row r="18" spans="1:6" s="11" customFormat="1">
       <c r="A18" s="10"/>
       <c r="C18" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="12"/>
       <c r="F18" s="12"/>
@@ -1243,294 +1793,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="4.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1">
-      <c r="A1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="90">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="45">
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="60">
-      <c r="B4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="45">
-      <c r="B5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="15" customFormat="1" ht="75">
-      <c r="B6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="8" spans="1:11" ht="75">
-      <c r="B8" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="75">
-      <c r="B9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="15" customFormat="1" ht="120">
-      <c r="C10" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" ht="45">
-      <c r="B11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="45">
-      <c r="B12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="60">
-      <c r="B13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="45">
-      <c r="B14" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="15" customFormat="1" ht="45">
-      <c r="B15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="H15" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="60">
-      <c r="B16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="45">
-      <c r="B17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="105">
-      <c r="C18" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="11">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Kosmetische Änderung für Präsentation
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_Anforderungsliste.xlsx
+++ b/Doku/Stundenplan_Anforderungsliste.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>Alle Daten werden in einer relationalen Datenbank gespeichert.</t>
   </si>
@@ -94,28 +94,10 @@
  - Bessere Trennung der einzelnen Komponenten.</t>
   </si>
   <si>
-    <t>Robustheit</t>
-  </si>
-  <si>
     <t>Bedienbarkeit</t>
   </si>
   <si>
     <t>Zeitverhalten</t>
-  </si>
-  <si>
-    <t>Verbrauchsverhalten</t>
-  </si>
-  <si>
-    <t>Analysierbarkeit</t>
-  </si>
-  <si>
-    <t>Stabilität</t>
-  </si>
-  <si>
-    <t>Testbarkeit</t>
-  </si>
-  <si>
-    <t>Koexistenz</t>
   </si>
   <si>
     <t>BUC1</t>
@@ -134,15 +116,6 @@
 - Installierbarkeit</t>
   </si>
   <si>
-    <t>Stromverbrauch?</t>
-  </si>
-  <si>
-    <t>Nutzung, Probleme?</t>
-  </si>
-  <si>
-    <t>Abstürze, Absturzursachen</t>
-  </si>
-  <si>
     <t>Das System muss dem Benutzer die Möglichkeit bieten die Planung manuell, durch Auswahl eines Feldes, als abgeschlossen zu markieren.</t>
   </si>
   <si>
@@ -253,9 +226,6 @@
     <t>Eine bestehende Planung wird automatisch überschrieben.</t>
   </si>
   <si>
-    <t>Das System soll eine automatische Planung auch ohne die Erfassung aller Zeitpräferenzen, jedoch mit mindestens einer Zeitpräferenz, ermöglichen.</t>
-  </si>
-  <si>
     <t>Das System kann eine Hinweismeldung ausgeben, falls eine Planung gestartet wird und nicht alle Dozenten die Zeitpräferenzen erfasst haben.</t>
   </si>
   <si>
@@ -296,9 +266,6 @@
     <t>Nur relevant wenn GAF "Planung manuell bearbeiten" aktiv ist.</t>
   </si>
   <si>
-    <t>Das System kann dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen und speichern.</t>
-  </si>
-  <si>
     <t>Das System sollte dem Benutzer die Möglichkeit bieten bereits erfasste Zeitpräferenzen eines Dozenten anzeigen und bearbeiten zu können.</t>
   </si>
   <si>
@@ -327,6 +294,12 @@
   </si>
   <si>
     <t>Sobald ein Benutzer das Planungsmodul aufruft, muss dieses innerhalb von 5 Sekunden vollständig zur Verfügung stehen.</t>
+  </si>
+  <si>
+    <t>Das System soll eine automatische Planung auch ohne die Erfassung aller Zeitpräferenzen ermöglichen.</t>
+  </si>
+  <si>
+    <t>Das System soll dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen und speichern.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -437,6 +410,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -503,7 +556,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -535,24 +588,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,13 +621,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -987,15 +1100,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.83203125" style="7" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="11" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" style="9" customWidth="1"/>
@@ -1008,443 +1121,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="75">
-      <c r="A2" s="20">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="15">
+        <v>5</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="75">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="15">
+        <v>5</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" ht="75">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="15">
+        <v>5</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" ht="45">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="15">
+        <v>3</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="60">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="15">
+        <v>2</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="45">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="45">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="15">
+        <v>5</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" ht="60">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="15">
+        <v>2</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" ht="60">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="15">
+        <v>3</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" ht="60">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="15">
+        <v>2</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="16" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" ht="45">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="60">
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="23" t="s">
+      <c r="D19" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="20">
-        <v>5</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" ht="75">
-      <c r="A3" s="20">
-        <v>2</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="20">
-        <v>5</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" ht="75">
-      <c r="A4" s="20">
-        <v>3</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="20">
-        <v>5</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="1:11" ht="45">
-      <c r="A5" s="20">
-        <v>4</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="20">
-        <v>3</v>
-      </c>
-      <c r="H5" s="20" t="s">
+      <c r="C20" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" ht="60">
-      <c r="A6" s="20">
-        <v>5</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="20">
-        <v>2</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" ht="45">
-      <c r="A7" s="20">
-        <v>6</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="21" t="s">
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="10" customFormat="1" ht="45">
+      <c r="A21" s="34"/>
+      <c r="B21" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="20">
-        <v>1</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" ht="45">
-      <c r="A8" s="20">
-        <v>7</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="20">
-        <v>5</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" ht="60">
-      <c r="A9" s="20">
-        <v>8</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="20">
-        <v>2</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" ht="60">
-      <c r="A10" s="20">
-        <v>9</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="20">
-        <v>3</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:11" ht="60">
-      <c r="A11" s="20">
-        <v>10</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="20">
-        <v>2</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" ht="45">
-      <c r="B16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="2:10" ht="45">
-      <c r="B17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="45">
-      <c r="C18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="60">
-      <c r="C19" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="45">
-      <c r="B20" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" s="10" customFormat="1" ht="45">
-      <c r="B21" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="105">
-      <c r="C22" s="13" t="s">
+    </row>
+    <row r="22" spans="1:10" ht="105">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="E22" s="41"/>
+      <c r="F22" s="44" t="s">
         <v>18</v>
       </c>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1470,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1484,155 +1619,155 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" ht="30">
-      <c r="A2" s="26">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" ht="60">
-      <c r="A3" s="26">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="22" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" s="7" customFormat="1" ht="75">
-      <c r="A4" s="26">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" s="7" customFormat="1" ht="30">
-      <c r="A5" s="26">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="30">
-      <c r="A6" s="26">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="30">
-      <c r="A7" s="26">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1">
       <c r="A8" s="6"/>
@@ -1646,68 +1781,48 @@
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1">
       <c r="A10" s="6"/>
-      <c r="C10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:11" s="7" customFormat="1">
       <c r="A11" s="6"/>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1">
       <c r="A12" s="6"/>
-      <c r="C12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1">
       <c r="A13" s="6"/>
-      <c r="C13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:11" s="7" customFormat="1">
       <c r="A14" s="6"/>
-      <c r="C14" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:11" s="7" customFormat="1">
       <c r="A15" s="6"/>
-      <c r="C15" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1">
       <c r="A16" s="6"/>
-      <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" s="7" customFormat="1">
       <c r="A17" s="6"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="F17" s="8"/>
     </row>
@@ -1815,8 +1930,8 @@
     </row>
     <row r="35" spans="1:6" s="7" customFormat="1">
       <c r="A35" s="6"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" s="2" customFormat="1">
@@ -1869,8 +1984,8 @@
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1">
       <c r="A44" s="4"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
       <c r="F44" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FCD Präsentation erstellt; EA-Modell angepasst
EA-Modell
-> Beschreibung der App-Functions
-> Fragen notiert
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_Anforderungsliste.xlsx
+++ b/Doku/Stundenplan_Anforderungsliste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="funktional" sheetId="2" r:id="rId1"/>
@@ -287,9 +287,6 @@
     <t>Das System muss einen Stundenplan, der nach Räumen sortiert ist, anzeigen.</t>
   </si>
   <si>
-    <t>Das System muss nach der Berechnung des Zuordnungsproblems eine zulässige Lösung in Form eines Stundenplans, selektiert nach Räumen, anzeigen.</t>
-  </si>
-  <si>
     <t>Ein Benutzer muss nach 10 minütiger Einarbeitungszeit in der Lage sein, die Zeitpräferenzen eines Dozenten zu erfassen.</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>Das System soll dem Benutzer die Möglichkeit bieten die Zeitpräferenzen eines Dozenten über vordefinierte Zeitblöcke (Wochenarbeitsstunden) zu erfassen und speichern.</t>
+  </si>
+  <si>
+    <t>Das System muss nach der Berechnung des Zuordnungsproblems eine zulässige Lösung in Form eines Stundenplans, selektiert nach Studiengängen, anzeigen.</t>
   </si>
 </sst>
 </file>
@@ -1100,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1190,7 +1190,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>56</v>
@@ -1271,7 +1271,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>51</v>
@@ -1354,7 +1354,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>69</v>
@@ -1605,7 +1605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>24</v>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Anforderungsliste um neuen GAF erweitert
</commit_message>
<xml_diff>
--- a/Doku/Stundenplan_Anforderungsliste.xlsx
+++ b/Doku/Stundenplan_Anforderungsliste.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>Alle Daten werden in einer relationalen Datenbank gespeichert.</t>
   </si>
@@ -68,19 +68,6 @@
   </si>
   <si>
     <t>Wichtigkeit (0 - 5)</t>
-  </si>
-  <si>
-    <t>Das System wird dem Benutzer keine Möglichkeit bieten die Stammdaten zu editieren.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Die Stammdaten der zu erfassenden Studiengänge, Räume oder Dozenten verändert sich nur geringfügig. Den Benutzern soll aus diesem Grund keine Anpassungs-möglichkeit gewährt werden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Das System darf keinen Eingabedialog auf Stammdaten zulassen.
- - Das System darf keinen schreibenden Zugriff auf Tabellen der Stammdaten gewähren.</t>
-  </si>
-  <si>
-    <t>Das System soll den Benutzer bei der Aufnahme einer Zeitpräferenz, welche bereits X-Mal vergeben wurde, warnen und Zeitvorschläge unterbreiten.</t>
   </si>
   <si>
     <t>Der Aufruf und die Bearbeitung des Stundenplanerstellungstools ist über einen beliebigen Browser möglich.</t>
@@ -106,9 +93,6 @@
     <t>Das System muss das mathematische Zuordnungsproblem der vorhandenen Informationen (Raum, Veranstaltung, Dozent inklusive Zeitpräferenz) mit Hilfe eines geeigneten Algorithmus automatisch berechnen.</t>
   </si>
   <si>
-    <t>Das System muss dem Benutzer die Möglichkeit gewähren jegliche Eingaben über die Tastatur oder die Maus vorzunehmen.</t>
-  </si>
-  <si>
     <t>Das System muss über einen Browser bedient und ausgeführt werden können.</t>
   </si>
   <si>
@@ -116,12 +100,6 @@
 - Installierbarkeit</t>
   </si>
   <si>
-    <t>Das System muss dem Benutzer die Möglichkeit bieten die Planung manuell, durch Auswahl eines Feldes, als abgeschlossen zu markieren.</t>
-  </si>
-  <si>
-    <t>Das System muss dem Benutzer bei Auswahl des Feldes "Planung abgeschlossen" eine Rückmeldung liefern, dass die Planung für das jeweilige Semester anschließend nicht mehr verändert werden kann.</t>
-  </si>
-  <si>
     <t>Das System soll einen entsprechenden Eingabedialog aufweisen.</t>
   </si>
   <si>
@@ -135,49 +113,10 @@
     <t xml:space="preserve"> - Eine manuelle Zuteilung der einzelnen Dozenten inklusive ihrer Zeitpräferenzen zu bestehenden Räumen und Modulen ist zu aufwendig und zu zeitintensiv</t>
   </si>
   <si>
-    <t>Das System soll dem Benutzer die Möglichkeit bieten den Stundenplan der aktuellen Semesterplanung manuell anzupassen.</t>
-  </si>
-  <si>
-    <t>Ein Dialog zur Änderung einzelner Blöcke.</t>
-  </si>
-  <si>
-    <t>Das System soll bei manueller Anpassung einzelner Blöcke mit anschließenden Kollisionen Zuordnungsvorschläge (Raum und Zeit) unterbreiten.</t>
-  </si>
-  <si>
     <t>Nach der Ausführung der automatischen Planung, muss über die Anzeige ein vollständiger Stundenplan aufrufbar sein.</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Um fehlerhafte Planungen zu korrigieren.</t>
-  </si>
-  <si>
-    <t>Button durch den eine bestehende Planung gelöscht wird.</t>
-  </si>
-  <si>
     <t>BUC4</t>
-  </si>
-  <si>
-    <t>Das System muss die Möglichkeit bieten, solange die Planung nicht als abgeschlossen markiert wurde, die gesamte Planung manuell zu löschen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Wenn das Semester begonnen hat, darf die Planung nicht mehr grundlegend verändert werden.</t>
-  </si>
-  <si>
-    <t>Button "Planung abschließen" der die Änderungen festschreibt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Einen versehentlichen Abschluss verhindern.</t>
-  </si>
-  <si>
-    <t>Rückmeldung vom System bevor der Abschluss gesetzt wird.</t>
-  </si>
-  <si>
-    <t>BUC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Einzelne Änderung auf Basis menschlicher Erkenntnisse.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Es können Zeiten oder Räume ausgewählt werden, die nicht zur Verfügung stehen.</t>
   </si>
   <si>
     <t xml:space="preserve"> - Dozenten lassen sich mit der Zeitvergabe Zeit.
@@ -211,12 +150,6 @@
     <t>Nach der manuellen Speicherung, müssen die betreffenden Daten aus der Datenbank auslesbar sein.</t>
   </si>
   <si>
-    <t>Nur relevant wenn GAF "Planung löschen" aktiv ist.</t>
-  </si>
-  <si>
-    <t>Nur relevant wenn Planung manuell abgeschlossen werden soll.</t>
-  </si>
-  <si>
     <t>Das System soll beim Start einer automatischen Planung eine bestehende Planung automatisch löschen.</t>
   </si>
   <si>
@@ -254,27 +187,9 @@
     <t>ID 8</t>
   </si>
   <si>
-    <t>Opionaler GAF</t>
-  </si>
-  <si>
-    <t>Optionaler GAF</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Es stehen nur begrenzte Räumlichkeiten zur Verfügung. </t>
-  </si>
-  <si>
-    <t>Nur relevant wenn GAF "Planung manuell bearbeiten" aktiv ist.</t>
-  </si>
-  <si>
     <t>Das System sollte dem Benutzer die Möglichkeit bieten bereits erfasste Zeitpräferenzen eines Dozenten anzeigen und bearbeiten zu können.</t>
   </si>
   <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>optionaler GAF</t>
-  </si>
-  <si>
     <t>BUC3</t>
   </si>
   <si>
@@ -300,13 +215,37 @@
   </si>
   <si>
     <t>Das System muss nach der Berechnung des Zuordnungsproblems eine zulässige Lösung in Form eines Stundenplans, selektiert nach Studiengängen, anzeigen.</t>
+  </si>
+  <si>
+    <t>Das System soll dem Benutzer vor der Durchführung einer Stundenplanberechnung einen Hinweis geben, dass evtl. bereits eine Planung vorhanden ist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Eine Planung muss bereits durchgeführt worden sein.</t>
+  </si>
+  <si>
+    <t>Das System muss nach dem Ausführen der Funktion "Stundenplan Löschen" die Stundenplaninformationen aus der Datenbank entfernen.</t>
+  </si>
+  <si>
+    <t>Das System muss dem Benutzer die Möglichkeit gewähren jegliche Eingaben über die Maus vorzunehmen.</t>
+  </si>
+  <si>
+    <t>Prüfung der Entwicklung auf Einhaltung der strikten Trennung der Komponenten.</t>
+  </si>
+  <si>
+    <t>Prüfung der Daten, die durch den Nutzer erfasst werden, und deren Speicherung in der Datenbank.</t>
+  </si>
+  <si>
+    <t>Probelauf mit Stoppuhr muss erfolgreich verlaufen.</t>
+  </si>
+  <si>
+    <t>Prüfung der Eingaben nach Abschluss der Entwicklungsarbeit.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,27 +290,6 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -387,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -410,86 +328,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -556,7 +394,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -619,90 +457,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1101,7 +855,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G26" sqref="G26:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1160,23 +914,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="18" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G2" s="15">
         <v>5</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -1187,23 +941,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="18" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="G3" s="15">
         <v>5</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -1214,23 +968,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="18" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G4" s="15">
         <v>5</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -1241,23 +995,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="18" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="G5" s="15">
         <v>3</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -1268,23 +1022,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="18" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="G6" s="15">
         <v>2</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -1295,23 +1049,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="18" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G7" s="15">
         <v>1</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -1325,23 +1079,23 @@
         <v>13</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="18" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="G8" s="15">
         <v>5</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -1354,23 +1108,23 @@
         <v>13</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G9" s="15">
         <v>2</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
@@ -1383,20 +1137,20 @@
         <v>13</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="18" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G10" s="15">
         <v>3</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
@@ -1407,189 +1161,83 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="18" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="G11" s="15">
         <v>2</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" ht="45">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="27"/>
-    </row>
-    <row r="17" spans="1:10" ht="45">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30" t="s">
+    <row r="12" spans="1:11" ht="90">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="60">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="31" t="s">
+      <c r="C12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="15">
+        <v>3</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="10" customFormat="1" ht="45">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="105">
-      <c r="A22" s="40"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="45"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="16" spans="1:11" s="10" customFormat="1"/>
+    <row r="17" spans="3:6">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="3:6" s="10" customFormat="1"/>
+    <row r="22" spans="3:6">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G20:I20"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1606,7 +1254,7 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1653,7 +1301,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="7" customFormat="1" ht="30">
+    <row r="2" spans="1:11" s="7" customFormat="1" ht="45">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -1662,11 +1310,15 @@
         <v>0</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2" s="15"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="15"/>
+      <c r="F2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="15">
+        <v>5</v>
+      </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -1678,16 +1330,18 @@
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="G3" s="15">
+        <v>5</v>
+      </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -1702,11 +1356,15 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" s="15"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="15"/>
+      <c r="F4" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="15">
+        <v>5</v>
+      </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
@@ -1718,14 +1376,18 @@
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="17" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E5" s="15"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="15">
+        <v>3</v>
+      </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
@@ -1737,14 +1399,16 @@
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="17" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="17"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="15">
+        <v>3</v>
+      </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -1756,13 +1420,15 @@
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="17" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>

</xml_diff>